<commit_message>
Fix: Add student import sample file with avatar column
</commit_message>
<xml_diff>
--- a/uef_diem_danh/uploadexcels/Student import sample.xlsx
+++ b/uef_diem_danh/uploadexcels/Student import sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmings\Project\Real projects\Diem_danh_nha_nuoc\real-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABE160-ADDD-480C-851E-82A6248CAB4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEB9AC8-1C3B-42CA-949C-F58E044C8AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DANH SÁCH HỌC SINH</t>
   </si>
@@ -68,12 +68,15 @@
 + Không được di chuyển vị trí các cột (có thể kéo rộng ra để có thể dễ xem)
 + Điền các thông tin cần thiết ở phía bên dưới mỗi cột</t>
   </si>
+  <si>
+    <t>Ảnh học viên</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +132,12 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,7 +200,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -385,16 +413,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}" name="Table1" displayName="Table1" ref="A3:G4" insertRow="1" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A3:G4" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A7B24D2D-7CB4-41CD-A03E-CC8EEA6A5C9B}" name="STT" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{94832C3C-18A2-4477-BD22-B25A14E46E14}" name="Họ" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{442BC115-712B-447F-BAAD-F8F6A91BD569}" name="Tên" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{FC13E029-59E3-42C5-A952-AD7D4E35FEFA}" name="Email" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{64AB7638-8F03-4246-9236-A46962E432AC}" name="Số điện thoại" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{998069BA-EFB3-4904-B66B-7AFA36162BD4}" name="Ngày sinh (dd/mm/yyyy)" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B4A74678-2ECC-4248-BA98-29A5C5ABD7EF}" name="Địa chỉ" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}" name="Table1" displayName="Table1" ref="A3:H4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A3:H4" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{A7B24D2D-7CB4-41CD-A03E-CC8EEA6A5C9B}" name="STT" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{94832C3C-18A2-4477-BD22-B25A14E46E14}" name="Họ" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{442BC115-712B-447F-BAAD-F8F6A91BD569}" name="Tên" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{FC13E029-59E3-42C5-A952-AD7D4E35FEFA}" name="Email" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{64AB7638-8F03-4246-9236-A46962E432AC}" name="Số điện thoại" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{998069BA-EFB3-4904-B66B-7AFA36162BD4}" name="Ngày sinh (dd/mm/yyyy)" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{B4A74678-2ECC-4248-BA98-29A5C5ABD7EF}" name="Địa chỉ" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{9340DEC2-4D8F-43EF-80FF-45BF1924D023}" name="Ảnh học viên" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -663,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,9 +705,10 @@
     <col min="4" max="4" width="25.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="36.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="33.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
@@ -726,8 +756,11 @@
       <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="124.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -744,6 +777,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A6" s="6"/>
@@ -753,6 +787,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
@@ -762,6 +797,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A8" s="6"/>
@@ -771,6 +807,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A9" s="6"/>
@@ -780,6 +817,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A10" s="6"/>
@@ -789,6 +827,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A11" s="6"/>
@@ -798,6 +837,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A12" s="6"/>
@@ -807,6 +847,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A13" s="6"/>
@@ -816,6 +857,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A14" s="6"/>
@@ -825,6 +867,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A15" s="6"/>
@@ -834,6 +877,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A16" s="6"/>
@@ -843,8 +887,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A17" s="6"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -852,8 +897,9 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A18" s="6"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -861,8 +907,9 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A19" s="6"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -870,8 +917,9 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A20" s="6"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -879,8 +927,9 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A21" s="6"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -888,8 +937,9 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A22" s="6"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -897,8 +947,9 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A23" s="6"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -906,8 +957,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A24" s="6"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -915,8 +967,9 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A25" s="6"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -924,8 +977,9 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A26" s="6"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -933,8 +987,9 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A27" s="6"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -942,8 +997,9 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A28" s="6"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -951,273 +1007,14 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A29" s="6"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A30" s="6"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A31" s="6"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A32" s="6"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A33" s="6"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A34" s="6"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A35" s="6"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A36" s="6"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A37" s="6"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A38" s="6"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A40" s="6"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A41" s="6"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A42" s="6"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A43" s="6"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A44" s="6"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A45" s="6"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A46" s="6"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A47" s="6"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A48" s="6"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A49" s="6"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A50" s="6"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A53" s="6"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A54" s="6"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A55" s="6"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A56" s="6"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A57" s="6"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="H28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Fix: Cannot find student image when update or delete and fix extract student date of birth in excel
</commit_message>
<xml_diff>
--- a/uef_diem_danh/uploadexcels/Student import sample.xlsx
+++ b/uef_diem_danh/uploadexcels/Student import sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmings\Project\Real projects\Diem_danh_nha_nuoc\real-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEB9AC8-1C3B-42CA-949C-F58E044C8AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97CF8E-2995-4E43-A9CC-BB15D6FADDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -76,7 +75,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +144,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -157,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -165,11 +175,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -184,9 +210,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -197,7 +227,8 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -219,121 +250,159 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="15"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -354,6 +423,26 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -692,13 +781,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="6" customWidth="1"/>
     <col min="2" max="3" width="13" style="1" customWidth="1"/>
@@ -706,35 +795,35 @@
     <col min="5" max="5" width="19.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="36.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="34.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="7"/>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
     </row>
     <row r="2" spans="1:14" ht="106.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" s="2" customFormat="1" ht="23.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -760,14 +849,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" ht="124.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="193.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A5" s="6"/>
@@ -809,206 +899,6 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A20" s="6"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A21" s="6"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A23" s="6"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A24" s="6"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A25" s="6"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A26" s="6"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A27" s="6"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A28" s="6"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>

</xml_diff>

<commit_message>
Change: Remove HinhAnh column and change into DonVi column in Student import sample excel file
</commit_message>
<xml_diff>
--- a/uef_diem_danh/uploadexcels/Student import sample.xlsx
+++ b/uef_diem_danh/uploadexcels/Student import sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97CF8E-2995-4E43-A9CC-BB15D6FADDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A92CE3-1E0C-4B30-AA9B-B22EFDCD8877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,17 +68,14 @@
 + Điền các thông tin cần thiết ở phía bên dưới mỗi cột</t>
   </si>
   <si>
-    <t>Ảnh học viên</t>
+    <t>Đơn vị</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
-  </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,14 +141,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -191,11 +180,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -210,13 +198,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -227,8 +217,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -272,6 +261,26 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -285,17 +294,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -308,16 +312,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -330,16 +330,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -352,16 +348,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -374,34 +366,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -422,8 +386,8 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -436,12 +400,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -502,7 +460,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}" name="Table1" displayName="Table1" ref="A3:H4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}" name="Table1" displayName="Table1" ref="A3:H4" insertRow="1" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A3:H4" xr:uid="{9B3673EE-E782-4004-9E8E-EB55A69E897A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A7B24D2D-7CB4-41CD-A03E-CC8EEA6A5C9B}" name="STT" dataDxfId="7"/>
@@ -512,7 +470,7 @@
     <tableColumn id="5" xr3:uid="{64AB7638-8F03-4246-9236-A46962E432AC}" name="Số điện thoại" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{998069BA-EFB3-4904-B66B-7AFA36162BD4}" name="Ngày sinh (dd/mm/yyyy)" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{B4A74678-2ECC-4248-BA98-29A5C5ABD7EF}" name="Địa chỉ" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{9340DEC2-4D8F-43EF-80FF-45BF1924D023}" name="Ảnh học viên" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{9340DEC2-4D8F-43EF-80FF-45BF1924D023}" name="Đơn vị" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -781,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,26 +760,26 @@
   <sheetData>
     <row r="1" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="7"/>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
     </row>
     <row r="2" spans="1:14" ht="106.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="23.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
@@ -849,17 +807,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" ht="193.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="11"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" s="3" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -869,7 +827,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -879,7 +837,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" s="3" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -889,7 +847,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="6"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -899,6 +857,31 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
+    <row r="9" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:14" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:N1"/>

</xml_diff>

<commit_message>
feat: Add missing favicon and fix incorrect render pagination after search
</commit_message>
<xml_diff>
--- a/uef_diem_danh/uploadexcels/Student import sample.xlsx
+++ b/uef_diem_danh/uploadexcels/Student import sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570E7CB2-DED1-46C9-B734-89FD639A1C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF03533-7A13-4930-9398-3DF488BD6747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,18 +236,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -272,8 +260,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -560,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -570,93 +574,93 @@
     <col min="2" max="2" width="20" style="8" customWidth="1"/>
     <col min="3" max="3" width="8" style="6" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25" style="23" customWidth="1"/>
     <col min="6" max="6" width="32.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="29.88671875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" style="9" customWidth="1"/>
     <col min="8" max="8" width="29.33203125" style="2" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="G1" s="18" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="24"/>
+      <c r="G1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" s="5" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="19" t="s">
         <v>12</v>
       </c>
     </row>
@@ -664,10 +668,10 @@
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
-      <c r="D7" s="14"/>
-      <c r="E7"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="22"/>
       <c r="F7"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="11"/>
       <c r="H7"/>
     </row>
     <row r="8" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -675,9 +679,9 @@
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
-      <c r="E8"/>
+      <c r="E8" s="22"/>
       <c r="F8"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="11"/>
       <c r="H8"/>
     </row>
     <row r="9" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -685,9 +689,9 @@
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9"/>
+      <c r="E9" s="22"/>
       <c r="F9"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="11"/>
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -695,9 +699,9 @@
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
-      <c r="E10"/>
+      <c r="E10" s="22"/>
       <c r="F10"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="11"/>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -705,9 +709,9 @@
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
-      <c r="E11"/>
+      <c r="E11" s="22"/>
       <c r="F11"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="11"/>
       <c r="H11"/>
     </row>
     <row r="12" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -715,9 +719,9 @@
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
-      <c r="E12"/>
+      <c r="E12" s="22"/>
       <c r="F12"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="11"/>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -725,9 +729,9 @@
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
-      <c r="E13"/>
+      <c r="E13" s="22"/>
       <c r="F13"/>
-      <c r="G13" s="15"/>
+      <c r="G13" s="11"/>
       <c r="H13"/>
     </row>
     <row r="14" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -735,9 +739,9 @@
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
-      <c r="E14"/>
+      <c r="E14" s="22"/>
       <c r="F14"/>
-      <c r="G14" s="15"/>
+      <c r="G14" s="11"/>
       <c r="H14"/>
     </row>
     <row r="15" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -745,9 +749,9 @@
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
-      <c r="E15"/>
+      <c r="E15" s="22"/>
       <c r="F15"/>
-      <c r="G15" s="15"/>
+      <c r="G15" s="11"/>
       <c r="H15"/>
     </row>
     <row r="16" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -755,9 +759,9 @@
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16"/>
+      <c r="E16" s="22"/>
       <c r="F16"/>
-      <c r="G16" s="15"/>
+      <c r="G16" s="11"/>
       <c r="H16"/>
     </row>
     <row r="17" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -765,9 +769,9 @@
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
-      <c r="E17"/>
+      <c r="E17" s="22"/>
       <c r="F17"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="11"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -775,9 +779,9 @@
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
-      <c r="E18"/>
+      <c r="E18" s="22"/>
       <c r="F18"/>
-      <c r="G18" s="15"/>
+      <c r="G18" s="11"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -785,9 +789,9 @@
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
-      <c r="E19"/>
+      <c r="E19" s="22"/>
       <c r="F19"/>
-      <c r="G19" s="15"/>
+      <c r="G19" s="11"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -795,9 +799,9 @@
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
-      <c r="E20"/>
+      <c r="E20" s="22"/>
       <c r="F20"/>
-      <c r="G20" s="15"/>
+      <c r="G20" s="11"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -805,9 +809,9 @@
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
-      <c r="E21"/>
+      <c r="E21" s="22"/>
       <c r="F21"/>
-      <c r="G21" s="15"/>
+      <c r="G21" s="11"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -815,9 +819,9 @@
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
-      <c r="E22"/>
+      <c r="E22" s="22"/>
       <c r="F22"/>
-      <c r="G22" s="15"/>
+      <c r="G22" s="11"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -825,9 +829,9 @@
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
-      <c r="E23"/>
+      <c r="E23" s="22"/>
       <c r="F23"/>
-      <c r="G23" s="15"/>
+      <c r="G23" s="11"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -835,9 +839,9 @@
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
-      <c r="E24"/>
+      <c r="E24" s="22"/>
       <c r="F24"/>
-      <c r="G24" s="15"/>
+      <c r="G24" s="11"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -845,9 +849,9 @@
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
-      <c r="E25"/>
+      <c r="E25" s="22"/>
       <c r="F25"/>
-      <c r="G25" s="15"/>
+      <c r="G25" s="11"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -855,9 +859,9 @@
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
-      <c r="E26"/>
+      <c r="E26" s="22"/>
       <c r="F26"/>
-      <c r="G26" s="15"/>
+      <c r="G26" s="11"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -865,9 +869,9 @@
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
-      <c r="E27"/>
+      <c r="E27" s="22"/>
       <c r="F27"/>
-      <c r="G27" s="15"/>
+      <c r="G27" s="11"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -875,9 +879,9 @@
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
-      <c r="E28"/>
+      <c r="E28" s="22"/>
       <c r="F28"/>
-      <c r="G28" s="15"/>
+      <c r="G28" s="11"/>
       <c r="H28"/>
     </row>
     <row r="29" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -885,9 +889,9 @@
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
-      <c r="E29"/>
+      <c r="E29" s="22"/>
       <c r="F29"/>
-      <c r="G29" s="15"/>
+      <c r="G29" s="11"/>
       <c r="H29"/>
     </row>
     <row r="30" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -895,9 +899,9 @@
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
-      <c r="E30"/>
+      <c r="E30" s="22"/>
       <c r="F30"/>
-      <c r="G30" s="15"/>
+      <c r="G30" s="11"/>
       <c r="H30"/>
     </row>
     <row r="31" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -905,9 +909,9 @@
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
-      <c r="E31"/>
+      <c r="E31" s="22"/>
       <c r="F31"/>
-      <c r="G31" s="15"/>
+      <c r="G31" s="11"/>
       <c r="H31"/>
     </row>
     <row r="32" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -915,9 +919,9 @@
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
-      <c r="E32"/>
+      <c r="E32" s="22"/>
       <c r="F32"/>
-      <c r="G32" s="15"/>
+      <c r="G32" s="11"/>
       <c r="H32"/>
     </row>
     <row r="33" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -925,9 +929,9 @@
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
-      <c r="E33"/>
+      <c r="E33" s="22"/>
       <c r="F33"/>
-      <c r="G33" s="15"/>
+      <c r="G33" s="11"/>
       <c r="H33"/>
     </row>
     <row r="34" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -935,9 +939,9 @@
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
-      <c r="E34"/>
+      <c r="E34" s="22"/>
       <c r="F34"/>
-      <c r="G34" s="15"/>
+      <c r="G34" s="11"/>
       <c r="H34"/>
     </row>
     <row r="35" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -945,9 +949,9 @@
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
-      <c r="E35"/>
+      <c r="E35" s="22"/>
       <c r="F35"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="11"/>
       <c r="H35"/>
     </row>
     <row r="36" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -955,9 +959,9 @@
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
-      <c r="E36"/>
+      <c r="E36" s="22"/>
       <c r="F36"/>
-      <c r="G36" s="15"/>
+      <c r="G36" s="11"/>
       <c r="H36"/>
     </row>
     <row r="37" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.35">
@@ -965,9 +969,9 @@
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
-      <c r="E37"/>
+      <c r="E37" s="22"/>
       <c r="F37"/>
-      <c r="G37" s="15"/>
+      <c r="G37" s="11"/>
       <c r="H37"/>
     </row>
   </sheetData>

</xml_diff>